<commit_message>
COLA test set results
</commit_message>
<xml_diff>
--- a/results/F1_charts.xlsx
+++ b/results/F1_charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\majikthise\MLP_Group_Project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1242074-26A1-4D86-85F7-F05FF6A18A8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD88BC7E-485F-4FD8-9851-FE8D2550114D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16905" windowHeight="11310" xr2:uid="{2F3F741A-CBA9-4CBB-A57F-C0FAE37D0066}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12225" windowHeight="1650" xr2:uid="{2F3F741A-CBA9-4CBB-A57F-C0FAE37D0066}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
   <si>
     <t>precision</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>COLA</t>
+  </si>
+  <si>
+    <t>TWITTER</t>
   </si>
 </sst>
 </file>
@@ -289,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -350,11 +353,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2594,6 +2604,746 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Shruti" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>COLA - test set f1_score</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Shruti" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>f1_score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-9F15-4796-BE7F-52AE86F2D946}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$39:$B$62</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B-medium</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>B-medium</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>B-medium</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>BERT</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>BERT</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>BERT</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Roberta</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Roberta</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Roberta</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Majority vote</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Straight avg</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Lime</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Shap</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Attn</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>IntGr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Lime + Shap + Attn + IntGr</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Lime</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Shap</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Attn</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>IntGr</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>Lime + Shap + Attn + IntGr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Constituent models</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Baseline Ensembles</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Interpretability Ensembles (modal vote)</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Interpretability Ensembles (wtd avg)</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$39:$I$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.82367400000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82795700000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83678799999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86406499999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.87225799999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86419800000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.87714700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81379299999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81379299999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.85606099999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.85931599999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.84331199999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82509999999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.82526900000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.83937799999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.853904</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87206300000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85678100000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.84955800000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.860792</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-9F15-4796-BE7F-52AE86F2D946}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="521015392"/>
+        <c:axId val="521013752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="521015392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Shruti" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521013752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="521013752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.92"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Shruti" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521015392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Shruti" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2714,6 +3464,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3721,6 +4511,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4264,15 +5557,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
+      <xdr:colOff>128587</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>328613</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>147638</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4302,15 +5595,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>547686</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>35718</xdr:rowOff>
+      <xdr:colOff>471486</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>566739</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>64293</xdr:rowOff>
+      <xdr:colOff>490539</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>159543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4332,6 +5625,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>209553</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{607211E4-82B4-45CE-B244-6FA24FAB9259}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4637,10 +5968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA924837-D6A1-46A1-96BD-520CDE0C3667}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4656,7 +5987,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="18" t="s">
@@ -5427,7 +6758,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="18" t="s">
@@ -5488,13 +6819,21 @@
       <c r="F39" s="6">
         <v>0.77039800000000003</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="6"/>
+      <c r="G39" s="5">
+        <v>0.73085299999999997</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.94350299999999998</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0.82367400000000002</v>
+      </c>
+      <c r="J39" s="6">
+        <v>0.72286799999999996</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="7" t="s">
         <v>4</v>
       </c>
@@ -5510,13 +6849,21 @@
       <c r="F40" s="10">
         <v>0.79696400000000001</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="10"/>
+      <c r="G40" s="9">
+        <v>0.789744</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0.87005600000000005</v>
+      </c>
+      <c r="I40" s="9">
+        <v>0.82795700000000005</v>
+      </c>
+      <c r="J40" s="10">
+        <v>0.751938</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="7" t="s">
         <v>4</v>
       </c>
@@ -5532,13 +6879,21 @@
       <c r="F41" s="10">
         <v>0.81024700000000005</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="10"/>
+      <c r="G41" s="9">
+        <v>0.77272700000000005</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0.91242900000000005</v>
+      </c>
+      <c r="I41" s="9">
+        <v>0.83678799999999998</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0.75581399999999999</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="7" t="s">
         <v>5</v>
       </c>
@@ -5554,13 +6909,21 @@
       <c r="F42" s="10">
         <v>0.82542700000000002</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="10"/>
+      <c r="G42" s="9">
+        <v>0.82519299999999995</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.90678000000000003</v>
+      </c>
+      <c r="I42" s="9">
+        <v>0.86406499999999997</v>
+      </c>
+      <c r="J42" s="10">
+        <v>0.80426399999999998</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="7" t="s">
         <v>5</v>
       </c>
@@ -5576,13 +6939,21 @@
       <c r="F43" s="10">
         <v>0.85958299999999999</v>
       </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="10"/>
+      <c r="G43" s="9">
+        <v>0.80284999999999995</v>
+      </c>
+      <c r="H43" s="9">
+        <v>0.95480200000000004</v>
+      </c>
+      <c r="I43" s="9">
+        <v>0.87225799999999998</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0.80813999999999997</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="7" t="s">
         <v>5</v>
       </c>
@@ -5598,13 +6969,21 @@
       <c r="F44" s="10">
         <v>0.87476299999999996</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="10"/>
+      <c r="G44" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.88983100000000004</v>
+      </c>
+      <c r="I44" s="9">
+        <v>0.86419800000000002</v>
+      </c>
+      <c r="J44" s="10">
+        <v>0.80813999999999997</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="7" t="s">
         <v>6</v>
       </c>
@@ -5620,13 +6999,21 @@
       <c r="F45" s="10">
         <v>0.86907000000000001</v>
       </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="10"/>
+      <c r="G45" s="9">
+        <v>0.82382100000000003</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0.93785300000000005</v>
+      </c>
+      <c r="I45" s="9">
+        <v>0.87714700000000001</v>
+      </c>
+      <c r="J45" s="10">
+        <v>0.81976700000000002</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="7" t="s">
         <v>6</v>
       </c>
@@ -5642,13 +7029,21 @@
       <c r="F46" s="10">
         <v>0.69259999999999999</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="10"/>
+      <c r="G46" s="9">
+        <v>0.68604699999999996</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9">
+        <v>0.81379299999999999</v>
+      </c>
+      <c r="J46" s="10">
+        <v>0.68604699999999996</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="7" t="s">
         <v>6</v>
       </c>
@@ -5664,10 +7059,18 @@
       <c r="F47" s="10">
         <v>0.69259999999999999</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="10"/>
+      <c r="G47" s="9">
+        <v>0.68604699999999996</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9">
+        <v>0.81379299999999999</v>
+      </c>
+      <c r="J47" s="10">
+        <v>0.68604699999999996</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
@@ -5688,13 +7091,21 @@
       <c r="F48" s="6">
         <v>0.81973399999999996</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="6"/>
+      <c r="G48" s="5">
+        <v>0.77397300000000002</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0.95762700000000001</v>
+      </c>
+      <c r="I48" s="5">
+        <v>0.85606099999999996</v>
+      </c>
+      <c r="J48" s="6">
+        <v>0.77907000000000004</v>
+      </c>
     </row>
     <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="7" t="s">
         <v>20</v>
       </c>
@@ -5708,7 +7119,7 @@
       <c r="J49" s="10"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="11" t="s">
         <v>8</v>
       </c>
@@ -5724,16 +7135,24 @@
       <c r="F50" s="10">
         <v>0.83301700000000001</v>
       </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
+      <c r="G50" s="9">
+        <v>0.77930999999999995</v>
+      </c>
+      <c r="H50" s="9">
+        <v>0.95762700000000001</v>
+      </c>
+      <c r="I50" s="9">
+        <v>0.85931599999999997</v>
+      </c>
+      <c r="J50" s="10">
+        <v>0.78488400000000003</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="4">
@@ -5748,14 +7167,22 @@
       <c r="F51" s="5">
         <v>0.80645199999999995</v>
       </c>
-      <c r="G51" s="4"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="6"/>
+      <c r="G51" s="4">
+        <v>0.76798100000000002</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0.93502799999999997</v>
+      </c>
+      <c r="I51" s="5">
+        <v>0.84331199999999995</v>
+      </c>
+      <c r="J51" s="6">
+        <v>0.76162799999999997</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24" t="s">
+      <c r="A52" s="25"/>
+      <c r="B52" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C52" s="8">
@@ -5770,14 +7197,22 @@
       <c r="F52" s="9">
         <v>0.79886100000000004</v>
       </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="10"/>
+      <c r="G52" s="8">
+        <v>0.78227800000000003</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.87288100000000002</v>
+      </c>
+      <c r="I52" s="9">
+        <v>0.82509999999999994</v>
+      </c>
+      <c r="J52" s="10">
+        <v>0.74612400000000001</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="25"/>
+      <c r="B53" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="8">
@@ -5792,14 +7227,22 @@
       <c r="F53" s="9">
         <v>0.78747599999999995</v>
       </c>
-      <c r="G53" s="8"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="10"/>
+      <c r="G53" s="8">
+        <v>0.78717899999999996</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0.867232</v>
+      </c>
+      <c r="I53" s="9">
+        <v>0.82526900000000003</v>
+      </c>
+      <c r="J53" s="10">
+        <v>0.748062</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24" t="s">
+      <c r="A54" s="25"/>
+      <c r="B54" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="8">
@@ -5814,14 +7257,22 @@
       <c r="F54" s="9">
         <v>0.81404200000000004</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="10"/>
+      <c r="G54" s="8">
+        <v>0.79545500000000002</v>
+      </c>
+      <c r="H54" s="9">
+        <v>0.88983100000000004</v>
+      </c>
+      <c r="I54" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="J54" s="10">
+        <v>0.76744199999999996</v>
+      </c>
     </row>
     <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24" t="s">
+      <c r="A55" s="25"/>
+      <c r="B55" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="8">
@@ -5836,14 +7287,22 @@
       <c r="F55" s="9">
         <v>0.81214399999999998</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="10"/>
+      <c r="G55" s="8">
+        <v>0.77990400000000004</v>
+      </c>
+      <c r="H55" s="9">
+        <v>0.92090399999999994</v>
+      </c>
+      <c r="I55" s="9">
+        <v>0.84455999999999998</v>
+      </c>
+      <c r="J55" s="10">
+        <v>0.76744199999999996</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="24" t="s">
+      <c r="A56" s="26"/>
+      <c r="B56" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="8">
@@ -5858,16 +7317,24 @@
       <c r="F56" s="9">
         <v>0.81783700000000004</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="10"/>
+      <c r="G56" s="8">
+        <v>0.77512000000000003</v>
+      </c>
+      <c r="H56" s="9">
+        <v>0.91525400000000001</v>
+      </c>
+      <c r="I56" s="9">
+        <v>0.83937799999999996</v>
+      </c>
+      <c r="J56" s="10">
+        <v>0.75968999999999998</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="8">
@@ -5882,14 +7349,22 @@
       <c r="F57" s="9">
         <v>0.82732399999999995</v>
       </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="10"/>
+      <c r="G57" s="8">
+        <v>0.770455</v>
+      </c>
+      <c r="H57" s="9">
+        <v>0.95762700000000001</v>
+      </c>
+      <c r="I57" s="9">
+        <v>0.853904</v>
+      </c>
+      <c r="J57" s="10">
+        <v>0.77519400000000005</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24" t="s">
+      <c r="A58" s="25"/>
+      <c r="B58" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="8">
@@ -5904,14 +7379,22 @@
       <c r="F58" s="9">
         <v>0.85199199999999997</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="10"/>
+      <c r="G58" s="8">
+        <v>0.81067999999999996</v>
+      </c>
+      <c r="H58" s="9">
+        <v>0.94350299999999998</v>
+      </c>
+      <c r="I58" s="9">
+        <v>0.87206300000000003</v>
+      </c>
+      <c r="J58" s="10">
+        <v>0.81007799999999996</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24" t="s">
+      <c r="A59" s="25"/>
+      <c r="B59" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="8">
@@ -5926,14 +7409,22 @@
       <c r="F59" s="9">
         <v>0.83111999999999997</v>
       </c>
-      <c r="G59" s="8"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="10"/>
+      <c r="G59" s="8">
+        <v>0.77701100000000001</v>
+      </c>
+      <c r="H59" s="9">
+        <v>0.95480200000000004</v>
+      </c>
+      <c r="I59" s="9">
+        <v>0.85678100000000001</v>
+      </c>
+      <c r="J59" s="10">
+        <v>0.78100800000000004</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24" t="s">
+      <c r="A60" s="25"/>
+      <c r="B60" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="8">
@@ -5948,14 +7439,22 @@
       <c r="F60" s="9">
         <v>0.82542700000000002</v>
       </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="10"/>
+      <c r="G60" s="8">
+        <v>0.76887899999999998</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0.94915300000000002</v>
+      </c>
+      <c r="I60" s="9">
+        <v>0.84955800000000004</v>
+      </c>
+      <c r="J60" s="10">
+        <v>0.76937999999999995</v>
+      </c>
     </row>
     <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24" t="s">
+      <c r="A61" s="25"/>
+      <c r="B61" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C61" s="8">
@@ -5970,14 +7469,22 @@
       <c r="F61" s="9">
         <v>0.82542700000000002</v>
       </c>
-      <c r="G61" s="8"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="10"/>
+      <c r="G61" s="8">
+        <v>0.76993199999999995</v>
+      </c>
+      <c r="H61" s="9">
+        <v>0.95480200000000004</v>
+      </c>
+      <c r="I61" s="9">
+        <v>0.85245899999999997</v>
+      </c>
+      <c r="J61" s="10">
+        <v>0.77325600000000005</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25" t="s">
+      <c r="A62" s="26"/>
+      <c r="B62" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C62" s="12">
@@ -5992,83 +7499,328 @@
       <c r="F62" s="13">
         <v>0.82922200000000001</v>
       </c>
-      <c r="G62" s="12"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="14"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="26"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="26"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="26"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="26"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="26"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="26"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" s="26"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="26"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="26"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" s="26"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" s="26"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="26"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="26"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="26"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="26"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="26"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="26"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="26"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="26"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="26"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="26"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="26"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="26"/>
+      <c r="G62" s="12">
+        <v>0.78554800000000002</v>
+      </c>
+      <c r="H62" s="13">
+        <v>0.95197699999999996</v>
+      </c>
+      <c r="I62" s="13">
+        <v>0.860792</v>
+      </c>
+      <c r="J62" s="14">
+        <v>0.78876000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C69" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="25"/>
+      <c r="B71" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="25"/>
+      <c r="B72" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="25"/>
+      <c r="B73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="10"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="25"/>
+      <c r="B74" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="10"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="25"/>
+      <c r="B76" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="10"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="25"/>
+      <c r="B77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="10"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="26"/>
+      <c r="B78" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
+      <c r="K79" s="28"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="25"/>
+      <c r="B80" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="10"/>
+      <c r="K80" s="28"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="26"/>
+      <c r="B81" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
+      <c r="K81" s="28"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
+      <c r="K82" s="28"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="25"/>
+      <c r="B83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="10"/>
+      <c r="K83" s="28"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="25"/>
+      <c r="B84" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="10"/>
+      <c r="K84" s="28"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="25"/>
+      <c r="B85" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="10"/>
+      <c r="K85" s="28"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="25"/>
+      <c r="B86" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="10"/>
+      <c r="K86" s="28"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="26"/>
+      <c r="B87" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="14"/>
+      <c r="K87" s="28"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="6"/>
+      <c r="K88" s="28"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="25"/>
+      <c r="B89" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="10"/>
+      <c r="K89" s="28"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="25"/>
+      <c r="B90" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="10"/>
+      <c r="K90" s="28"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="25"/>
+      <c r="B91" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="10"/>
+      <c r="K91" s="28"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="25"/>
+      <c r="B92" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="10"/>
+      <c r="K92" s="28"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="26"/>
+      <c r="B93" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="14"/>
+      <c r="K93" s="28"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="28"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K95" s="28"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="28"/>
+    </row>
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="28"/>
+    </row>
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="28"/>
+    </row>
+    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K99" s="28"/>
+    </row>
+    <row r="100" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K100" s="28"/>
+    </row>
+    <row r="101" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K101" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="C80:H91">
-    <sortCondition ref="H80"/>
+  <sortState ref="K90:P101">
+    <sortCondition ref="P90"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="C37:F37"/>

</xml_diff>